<commit_message>
Update libraries and matching table balancesheet
</commit_message>
<xml_diff>
--- a/data/standardized_balancesheet.xlsx
+++ b/data/standardized_balancesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DE3116-3AD7-E143-A2EC-9E2B98261585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF3B305-04C5-784F-A9A4-ECED087E53AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25500" windowHeight="17860" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
@@ -36,188 +36,83 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
   <si>
     <t>standardized_balancesheet_label</t>
   </si>
   <si>
-    <t>standardized_balancesheet_Long_Description_std</t>
-  </si>
-  <si>
-    <t>Cash and cash equivalents include cash on hand and deposits with original maturities of three months or less. Marketable securities are highly liquid investments that can be quickly converted to cash.</t>
-  </si>
-  <si>
     <t>Total Accounts Receivable</t>
   </si>
   <si>
-    <t>Total amount owed to the entity by its customers for goods or services sold on credit, after considering any allowance for credit loss.</t>
-  </si>
-  <si>
     <t>Total Inventories</t>
   </si>
   <si>
-    <t>The cost of goods held by the entity for resale and materials used in production, reported at the lower of cost or market value.</t>
-  </si>
-  <si>
     <t>Other Current assets (to balance out the Total Current Assets)</t>
   </si>
   <si>
-    <t>Miscellaneous current assets not explicitly mentioned, balancing out the total current assets.</t>
-  </si>
-  <si>
     <t>Total Current Assets</t>
   </si>
   <si>
-    <t>The sum of cash, accounts receivable, inventories, and other current assets, representing assets expected to be converted into cash or used up within one year.</t>
-  </si>
-  <si>
     <t>Property, Plant and Equipment</t>
   </si>
   <si>
-    <t>The net book value of physical assets such as land, buildings, and machinery, less accumulated depreciation.</t>
-  </si>
-  <si>
-    <t>Long-term investments and advances made by the entity, typically in securities or other companies.</t>
-  </si>
-  <si>
     <t>Intangible Assets (excl. goodwill)</t>
   </si>
   <si>
-    <t>Non-physical assets, such as patents and copyrights, having a finite useful life and excluding goodwill.</t>
-  </si>
-  <si>
     <t>Goodwill</t>
   </si>
   <si>
-    <t>The excess of the purchase price over the fair value of identifiable net assets acquired in a business combination.</t>
-  </si>
-  <si>
     <t>Other Long Term Assets (to balance out the Total Long-Term Assets)</t>
   </si>
   <si>
-    <t>Miscellaneous long-term assets not explicitly mentioned, balancing out the total long-term assets.</t>
-  </si>
-  <si>
     <t>Total Long Term Assets</t>
   </si>
   <si>
-    <t>The sum of property, plant, equipment, long-term investments, intangible assets, and other long-term assets.</t>
-  </si>
-  <si>
     <t>Accounts Payable</t>
   </si>
   <si>
-    <t>Amounts owed by the entity to its suppliers and vendors for goods and services received on credit.</t>
-  </si>
-  <si>
     <t>Tax Payable</t>
   </si>
   <si>
-    <t>Taxes owed by the entity but not yet paid, including both current and deferred tax liabilities.</t>
-  </si>
-  <si>
-    <t>Other Account Payable (to balance out the Total Accounts Payable)</t>
-  </si>
-  <si>
-    <t>Miscellaneous payables and liabilities not explicitly mentioned, balancing out the total accounts payable.</t>
-  </si>
-  <si>
-    <t>Total Accounts Payable</t>
-  </si>
-  <si>
-    <t>The sum of amounts owed by the entity to its suppliers and vendors, representing current liabilities.</t>
-  </si>
-  <si>
-    <t>Short-Term Debt &amp; Capital Leasing</t>
-  </si>
-  <si>
-    <t>Short-term borrowings and obligations under capital leases that are due within one year.</t>
-  </si>
-  <si>
-    <t>Deferred Tax And Revenue</t>
-  </si>
-  <si>
-    <t>Deferred tax liabilities and revenue recognized for transactions that have been deferred for accounting purposes.</t>
-  </si>
-  <si>
     <t>Other Current Liabilities (to balance out the Total Current Liabilities)</t>
   </si>
   <si>
-    <t>Miscellaneous current liabilities not explicitly mentioned, balancing out the total current liabilities.</t>
-  </si>
-  <si>
     <t>Total Current Liabilities</t>
   </si>
   <si>
-    <t>The sum of all obligations that are expected to be settled within one year, including accounts payable, short-term debt, and other current liabilities.</t>
-  </si>
-  <si>
     <t>Long-Term Debts and Capital Leasing</t>
   </si>
   <si>
-    <t>Long-term borrowings and obligations under capital leases that are due beyond one year.</t>
-  </si>
-  <si>
     <t>Other Long-term liabilities (to balance out the total Long-term liabilities)</t>
   </si>
   <si>
-    <t>Miscellaneous long-term liabilities not explicitly mentioned, balancing out the total long-term liabilities.</t>
-  </si>
-  <si>
     <t>Total Long-Term liabilities</t>
   </si>
   <si>
-    <t>The sum of long-term debts, obligations under capital leases, and other long-term liabilities.</t>
-  </si>
-  <si>
     <t>Common Stock</t>
   </si>
   <si>
-    <t>The par or stated value of common stock issued by the entity to its shareholders.</t>
-  </si>
-  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
-    <t>Accumulated earnings retained by the entity, representing the portion of net income not distributed as dividends.</t>
-  </si>
-  <si>
     <t>Accumulated other comprehensive income (loss)</t>
   </si>
   <si>
-    <t>The cumulative change in equity from transactions and events outside the ordinary operations of the entity, such as foreign currency translation adjustments and unrealized gains or losses on certain investments.</t>
-  </si>
-  <si>
     <t>Additional paid-in capital</t>
   </si>
   <si>
-    <t>The excess of amounts paid by shareholders over the par value of common stock, representing contributed capital.</t>
-  </si>
-  <si>
     <t>Other stockholders Equity (to balance out the Total Stockholders Equity)</t>
   </si>
   <si>
-    <t>Miscellaneous equity items not explicitly mentioned, balancing out the total stockholders' equity.</t>
-  </si>
-  <si>
     <t>Total Stockholders Equity</t>
   </si>
   <si>
-    <t>The residual interest in the assets of the entity after deducting liabilities, including common stock, retained earnings, and additional paid-in capital.</t>
-  </si>
-  <si>
     <t>Minority interest</t>
   </si>
   <si>
-    <t>The portion of equity in a subsidiary not attributable to the parent company, representing the interest of minority shareholders.</t>
-  </si>
-  <si>
     <t>Total Equity</t>
   </si>
   <si>
-    <t>The sum of total stockholders' equity and minority interest, representing the total ownership interest in the entity.</t>
-  </si>
-  <si>
     <t>df_Facts_label</t>
   </si>
   <si>
@@ -242,9 +137,6 @@
     <t>Cash and Cash Equivalents, at Carrying Value</t>
   </si>
   <si>
-    <t xml:space="preserve"> Marketable Securities, Current</t>
-  </si>
-  <si>
     <t>Marketable Securities, Current</t>
   </si>
   <si>
@@ -258,6 +150,90 @@
   </si>
   <si>
     <t>Assets, Noncurrent - (Marketable Securities, Noncurrent + Property, Plant and Equipment, Net + Property, Plant and Equipment, Net + Goodwill)</t>
+  </si>
+  <si>
+    <t>Amount of currency on hand as well as demand deposits with banks or financial institutions. Includes other kinds of accounts that have the general characteristics of demand deposits. Also includes short-term, highly liquid investments that are both readily convertible to known amounts of cash and so near their maturity that they present insignificant risk of changes in value because of changes in interest rates. Excludes cash and cash equivalents within disposal group and discontinued operation.</t>
+  </si>
+  <si>
+    <t>df_Fact_Description</t>
+  </si>
+  <si>
+    <t>Marketable Securities, Current Amount of investment in marketable security, classified as current.</t>
+  </si>
+  <si>
+    <t>Amount, after allowance for credit loss, of right to consideration from customer for product sold and service rendered in normal course of business, classified as current.</t>
+  </si>
+  <si>
+    <t>Amount after valuation and LIFO reserves of inventory expected to be sold, or consumed within one year or operating cycle, if longer</t>
+  </si>
+  <si>
+    <t>Sum of the carrying amounts as of the balance sheet date of all assets that are expected to be realized in cash, sold, or consumed within one year (or the normal operating cycle, if longer). Assets are probable future economic benefits obtained or controlled by an entity as a result of past transactions or events.</t>
+  </si>
+  <si>
+    <t>Amount of investment in marketable security, classified as noncurrent.</t>
+  </si>
+  <si>
+    <t>Amount after accumulated depreciation, depletion and amortization of physical assets used in the normal conduct of business to produce goods and services and not intended for resale. Examples include, but are not limited to, land, buildings, machinery and equipment, office equipment, and furniture and fixtures.</t>
+  </si>
+  <si>
+    <t>Sum of the carrying amounts of all intangible assets, excluding goodwill, as of the balance sheet date, net of accumulated amortization and impairment charges.</t>
+  </si>
+  <si>
+    <t>Amount after accumulated impairment loss of an asset representing future economic benefits arising from other assets acquired in a business combination that are not individually identified and separately recognized.</t>
+  </si>
+  <si>
+    <t>Sum of the carrying amounts as of the balance sheet date of all assets that are expected to be realized in cash, sold or consumed after one year or beyond the normal operating cycle, if longer.</t>
+  </si>
+  <si>
+    <t>Carrying value as of the balance sheet date of liabilities incurred (and for which invoices have typically been received) and payable to vendors for goods and services received that are used in an entity's business. Used to reflect the current portion of the liabilities (due within one year or within the normal operating cycle if longer)</t>
+  </si>
+  <si>
+    <t>Accounts Payable, Current</t>
+  </si>
+  <si>
+    <t>Taxes Payable, Current</t>
+  </si>
+  <si>
+    <t>Carrying value as of the balance sheet date of obligations incurred and payable for statutory income, sales, use, payroll, excise, real, property and other taxes. Used to reflect the current portion of the liabilities (due within one year or within the normal operating cycle if longer).</t>
+  </si>
+  <si>
+    <t>Commercial papers</t>
+  </si>
+  <si>
+    <t>Short-Term Debt</t>
+  </si>
+  <si>
+    <t>Commercial Paper</t>
+  </si>
+  <si>
+    <t>Carrying value as of the balance sheet date of short-term borrowings using unsecured obligations issued by banks, corporations and other borrowers to investors. The maturities of these money market securities generally do not exceed 270 days</t>
+  </si>
+  <si>
+    <t>Long-term Debt, Current Maturities</t>
+  </si>
+  <si>
+    <t>Amount, after unamortized (discount) premium and debt issuance costs, of long-term debt, classified as current. Includes, but not limited to, notes payable, bonds payable, debentures, mortgage loans and commercial paper. Excludes capital lease obligations</t>
+  </si>
+  <si>
+    <t>Operating Lease, Liability, Current</t>
+  </si>
+  <si>
+    <t>Finance Lease, Liability, Current</t>
+  </si>
+  <si>
+    <t>Present value of lessee's discounted obligation for lease payments from finance lease, classified as current.</t>
+  </si>
+  <si>
+    <t>Present value of lessee's discounted obligation for lease payments from operating lease, classified as current.</t>
+  </si>
+  <si>
+    <t>Liabilities, Current</t>
+  </si>
+  <si>
+    <t>Total obligations incurred as part of normal operations that are expected to be paid during the following twelve months or within one business cycle, if longer.</t>
+  </si>
+  <si>
+    <t>Liabilities, Current - (Accounts Payable, Current + Taxes Payable, Current + Commercial Paper + Long-term Debt, Current Maturities + Operating Lease, Current + Finance Lease, Liability, Current)</t>
   </si>
 </sst>
 </file>
@@ -352,8 +328,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -672,15 +648,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="62.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="83.1640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="65.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -689,303 +665,297 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="G1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="3" t="s">
-        <v>37</v>
+        <v>13</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>39</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>43</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>47</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="B29" s="4"/>
-      <c r="C29" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>57</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="C32" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update matching table balancesheet
</commit_message>
<xml_diff>
--- a/data/standardized_balancesheet.xlsx
+++ b/data/standardized_balancesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF3B305-04C5-784F-A9A4-ECED087E53AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C18EF5B-742B-9D4D-A9A5-056CD1716978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25500" windowHeight="17860" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="101">
   <si>
     <t>standardized_balancesheet_label</t>
   </si>
@@ -80,39 +80,24 @@
     <t>Total Current Liabilities</t>
   </si>
   <si>
-    <t>Long-Term Debts and Capital Leasing</t>
-  </si>
-  <si>
     <t>Other Long-term liabilities (to balance out the total Long-term liabilities)</t>
   </si>
   <si>
     <t>Total Long-Term liabilities</t>
   </si>
   <si>
-    <t>Common Stock</t>
-  </si>
-  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
     <t>Accumulated other comprehensive income (loss)</t>
   </si>
   <si>
-    <t>Additional paid-in capital</t>
-  </si>
-  <si>
     <t>Other stockholders Equity (to balance out the Total Stockholders Equity)</t>
   </si>
   <si>
-    <t>Total Stockholders Equity</t>
-  </si>
-  <si>
     <t>Minority interest</t>
   </si>
   <si>
-    <t>Total Equity</t>
-  </si>
-  <si>
     <t>df_Facts_label</t>
   </si>
   <si>
@@ -234,13 +219,133 @@
   </si>
   <si>
     <t>Liabilities, Current - (Accounts Payable, Current + Taxes Payable, Current + Commercial Paper + Long-term Debt, Current Maturities + Operating Lease, Current + Finance Lease, Liability, Current)</t>
+  </si>
+  <si>
+    <t>Long-term Debt, Excluding Current Maturities</t>
+  </si>
+  <si>
+    <t>Long-Term Debts</t>
+  </si>
+  <si>
+    <t>Operating Lease, Liability, Non Current</t>
+  </si>
+  <si>
+    <t>Amount after unamortized (discount) premium and debt issuance costs of long-term debt classified as noncurrent and excluding amounts to be repaid within one year or the normal operating cycle, if longer. Includes, but not limited to, notes payable, bonds payable, debentures, mortgage loans and commercial paper. Excludes capital lease obligation</t>
+  </si>
+  <si>
+    <t>Finance Lease, Liability, Non Current</t>
+  </si>
+  <si>
+    <t>Operating Lease, Liability, Noncurrent</t>
+  </si>
+  <si>
+    <t>Present value of lessee's discounted obligation for lease payments from operating lease, classified as noncurrent.</t>
+  </si>
+  <si>
+    <t>Present value of lessee's discounted obligation for lease payments from finance lease, classified as noncurrent.</t>
+  </si>
+  <si>
+    <t>Total Assets</t>
+  </si>
+  <si>
+    <t>Sum of the carrying amounts as of the balance sheet date of all assets that are recognized. Assets are probable future economic benefits obtained or controlled by an entity as a result of past transactions or events</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>Liabilities, Noncurrent</t>
+  </si>
+  <si>
+    <t>Liabilities</t>
+  </si>
+  <si>
+    <t>Total Liabilities</t>
+  </si>
+  <si>
+    <t>Sum of the carrying amounts as of the balance sheet date of all liabilities that are recognized. Liabilities are probable future sacrifices of economic benefits arising from present obligations of an entity to transfer assets or provide services to other entities in the future.</t>
+  </si>
+  <si>
+    <t>Amount of obligation due after one year or beyond the normal operating cycle, if longer.</t>
+  </si>
+  <si>
+    <t>Common Stocks, Including Additional Paid in Capital</t>
+  </si>
+  <si>
+    <t>Retained Earnings (Accumulated Deficit)</t>
+  </si>
+  <si>
+    <t>Accumulated Other Comprehensive Income (Loss), Net of Tax</t>
+  </si>
+  <si>
+    <t>Liabilities and Equity</t>
+  </si>
+  <si>
+    <t>Stockholders' Equity Attributable to Noncontrolling Interest</t>
+  </si>
+  <si>
+    <t>Total of all stockholders' equity (deficit) items, net of receivables from officers, directors, owners, and affiliates of the entity which is directly or indirectly attributable to that ownership interest in subsidiary equity which is not attributable to the parent (that is, noncontrolling interest, previously referred to as minority interest).</t>
+  </si>
+  <si>
+    <t>Preferred Stock</t>
+  </si>
+  <si>
+    <t>Total Company Equity</t>
+  </si>
+  <si>
+    <t>Total Stockholders' Equity</t>
+  </si>
+  <si>
+    <t>Preferred Stock, Shares Authorized</t>
+  </si>
+  <si>
+    <t>Total Liabilities, preferred stock &amp; Stockholders' Equity</t>
+  </si>
+  <si>
+    <t>Liabilities and Equity - Liabilities</t>
+  </si>
+  <si>
+    <t>Liabilities and Equity - ( Liabilities + Stockholders' Equity Attributable to Noncontrolling Interest)</t>
+  </si>
+  <si>
+    <t>Liabilities and Equity - ( Liabilities + Stockholders' Equity Attributable to Noncontrolling Interest + Accumulated Other Comprehensive Income (Loss), Net of Tax + Retained Earnings (Accumulated Deficit) + Preferred Stock, Shares Authorized + Common Stocks, Including Additional Paid in Capital )</t>
+  </si>
+  <si>
+    <t>Common Stock, Value, Issued</t>
+  </si>
+  <si>
+    <t>Additional Paid in Capital</t>
+  </si>
+  <si>
+    <t>Common Stock &amp; Additional paid-in capital (or)</t>
+  </si>
+  <si>
+    <t>Aggregate par or stated value of issued nonredeemable common stock (or common stock redeemable solely at the option of the issuer). This item includes treasury stock repurchased by the entity. Note: elements for number of nonredeemable common shares, par value and other disclosure concepts are in another section within stockholders' equity</t>
+  </si>
+  <si>
+    <t>Excess of issue price over par or stated value of the entity's capital stock and amounts received from other transactions involving the entity's stock or stockholders. Includes adjustments to additional paid in capital. Some examples of such adjustments include recording the issuance of debt with a beneficial conversion feature and certain tax consequences of equity instruments awarded to employees. Use this element for the aggregate amount of additional paid-in capital associated with common and preferred stock. For additional paid-in capital associated with only common stock, use the element additional paid in capital, common stock. For additional paid-in capital associated with only preferred stock, use the element additional paid in capital, preferred stock.</t>
+  </si>
+  <si>
+    <t>The maximum number of nonredeemable preferred shares (or preferred stock redeemable solely at the option of the issuer) permitted to be issued by an entity's charter and bylaws.</t>
+  </si>
+  <si>
+    <t>The cumulative amount of the reporting entity's undistributed earnings or deficit.</t>
+  </si>
+  <si>
+    <t>Liabilities, Noncurrent - ( Long-term Debt, Excluding Current Maturities + Operating Lease, Liability, Noncurrent + Finance Lease, Liability, Current)</t>
+  </si>
+  <si>
+    <t>Accumulated change in equity from transactions and other events and circumstances from non-owner sources, net of tax effect, at period end. Excludes Net Income (Loss), and accumulated changes in equity from transactions resulting from investments by owners and distributions to owners. Includes foreign currency translation items, certain pension adjustments, unrealized gains and losses on certain investments in debt and equity securities, other than temporary impairment (OTTI) losses related to factors other than credit losses on available-for-sale and held-to-maturity debt securities that an entity does not intend to sell and it is not more likely than not that the entity will be required to sell before recovery of the amortized cost basis, as well as changes in the fair value of derivatives related to the effective portion of a designated cash flow hedge</t>
+  </si>
+  <si>
+    <t>Amount of liabilities and equity items, including the portion of equity attributable to noncontrolling interests, if any.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -270,6 +375,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -313,7 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -323,12 +441,21 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -646,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -665,297 +792,415 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="C11" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="6" t="s">
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="C17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="3" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="B19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="B25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="B26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="B27" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="B33" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="B34" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="B35" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="6"/>
+      <c r="B37" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
balancesheet_std function: pivot wider & render
Build historical standardized balance sheet. Published.
</commit_message>
<xml_diff>
--- a/data/standardized_balancesheet.xlsx
+++ b/data/standardized_balancesheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C18EF5B-742B-9D4D-A9A5-056CD1716978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E896C2B-2863-2949-83E4-E0C6B3E94D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25500" windowHeight="17860" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
+    <workbookView xWindow="24400" yWindow="600" windowWidth="26800" windowHeight="20500" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2_Calculated_Fields" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="101">
   <si>
     <t>standardized_balancesheet_label</t>
   </si>
@@ -116,9 +117,6 @@
     <t>Property, Plant and Equipment, Net</t>
   </si>
   <si>
-    <t>Cash, Cash Equivalent</t>
-  </si>
-  <si>
     <t>Cash and Cash Equivalents, at Carrying Value</t>
   </si>
   <si>
@@ -339,6 +337,9 @@
   </si>
   <si>
     <t>Amount of liabilities and equity items, including the portion of equity attributable to noncontrolling interests, if any.</t>
+  </si>
+  <si>
+    <t>Cash &amp; Cash Equivalent</t>
   </si>
 </sst>
 </file>
@@ -431,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -445,9 +446,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -773,17 +771,398 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="62.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="83.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="83.1640625" style="3" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="65.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C505A6-D873-2541-9A06-08B0F1ED3661}">
+  <dimension ref="A1:G39"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="62.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="83.1640625" style="3" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="65.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -795,31 +1174,31 @@
         <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -830,7 +1209,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -841,7 +1220,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -857,22 +1236,22 @@
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -883,7 +1262,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -891,10 +1270,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -905,7 +1284,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -913,7 +1292,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="5"/>
     </row>
@@ -921,11 +1300,11 @@
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>31</v>
+      <c r="B13" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -933,10 +1312,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -944,54 +1323,54 @@
         <v>11</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -999,63 +1378,63 @@
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="8" t="s">
+      <c r="A23" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="B23" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="C23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1063,7 +1442,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C26" s="5"/>
     </row>
@@ -1071,64 +1450,64 @@
       <c r="A27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>72</v>
+      <c r="B27" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1136,10 +1515,10 @@
         <v>16</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1147,10 +1526,10 @@
         <v>17</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1158,16 +1537,16 @@
         <v>18</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" s="5"/>
     </row>
@@ -1176,30 +1555,30 @@
         <v>19</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>80</v>
+        <v>86</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bs_std: WIP to add appropriate rows of missing elements
</commit_message>
<xml_diff>
--- a/data/standardized_balancesheet.xlsx
+++ b/data/standardized_balancesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/Documents/Github/SEC_data_analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C612021-1AA0-704E-93B0-070A5242D558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB59C8FA-E211-C04C-9A07-B380C03987BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16700" yWindow="860" windowWidth="17500" windowHeight="19980" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
+    <workbookView xWindow="25920" yWindow="5340" windowWidth="17500" windowHeight="19980" activeTab="1" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -785,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -1190,7 +1190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C505A6-D873-2541-9A06-08B0F1ED3661}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bs_std: cleaning the df. New render
Cleaning dataframe. Addressing instances in which the filing includes comparison with previous reporting period. (WIP). New rendering structure.
</commit_message>
<xml_diff>
--- a/data/standardized_balancesheet.xlsx
+++ b/data/standardized_balancesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB59C8FA-E211-C04C-9A07-B380C03987BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6D0FD0-C379-714F-B7FD-34B981B5B91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25920" yWindow="5340" windowWidth="17500" windowHeight="19980" activeTab="1" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
+    <workbookView xWindow="16060" yWindow="5140" windowWidth="17500" windowHeight="19980" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="101">
   <si>
     <t>standardized_balancesheet_label</t>
   </si>
@@ -337,18 +337,6 @@
   </si>
   <si>
     <t>Other Stockholders Equity (to balance out the Total Stockholders Equity)</t>
-  </si>
-  <si>
-    <t>Preferred Stock, Value, Issued</t>
-  </si>
-  <si>
-    <t>Temporary Equity, Carrying Amount, Attributable to Parent</t>
-  </si>
-  <si>
-    <t>Total number of nonredeemable preferred shares (or preferred stock redeemable solely at the option of the issuer) issued to shareholders (includes related preferred shares that were issued, repurchased, and remain in the treasury). May be all or portion of the number of preferred shares authorized. Excludes preferred shares that are classified as debt.</t>
-  </si>
-  <si>
-    <t>Carrying amount, attributable to parent, of an entity's issued and outstanding stock which is not included within permanent equity. Temporary equity is a security with redemption features that are outside the control of the issuer, is not classified as an asset or liability in conformity with GAAP, and is not mandatorily redeemable. Includes any type of security that is redeemable at a fixed or determinable price or on a fixed or determinable date or dates, is redeemable at the option of the holder, or has conditions for redemption which are not solely within the control of the issuer. Includes stock with a put option held by an ESOP and stock redeemable by a holder only in the event of a change in control of the issuer.</t>
   </si>
   <si>
     <t>Amount of stockholders' equity (deficit), net of receivables from officers, directors, owners, and affiliates of the entity, attributable to both the parent and noncontrolling interests. Amount excludes temporary equity. Alternate caption for the concept is permanent equity.</t>
@@ -783,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1070,116 +1058,72 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>53</v>
+    </row>
+    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1190,7 +1134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C505A6-D873-2541-9A06-08B0F1ED3661}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bs_std finalized with missing data
change approach to finalize bs_std
</commit_message>
<xml_diff>
--- a/data/standardized_balancesheet.xlsx
+++ b/data/standardized_balancesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/Documents/Github/SEC_data_analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25CBE4F-E9F7-124B-BD8E-87F6D7A02195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922CA847-DB31-5D4F-816F-BEAFE993D958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22420" yWindow="860" windowWidth="11140" windowHeight="19980" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
+    <workbookView xWindow="3080" yWindow="1600" windowWidth="21120" windowHeight="19980" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
   <si>
     <t>standardized_balancesheet_label</t>
   </si>
@@ -47,18 +47,12 @@
     <t>Total Current Assets</t>
   </si>
   <si>
-    <t>Property, Plant and Equipment</t>
-  </si>
-  <si>
     <t>Intangible Assets (excl. goodwill)</t>
   </si>
   <si>
     <t>Goodwill</t>
   </si>
   <si>
-    <t>Total Long Term Assets</t>
-  </si>
-  <si>
     <t>Accounts Payable</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>Amount, after allowance for credit loss, of right to consideration from customer for product sold and service rendered in normal course of business, classified as current.</t>
   </si>
   <si>
-    <t>Amount after valuation and LIFO reserves of inventory expected to be sold, or consumed within one year or operating cycle, if longer</t>
-  </si>
-  <si>
     <t>Sum of the carrying amounts as of the balance sheet date of all assets that are expected to be realized in cash, sold, or consumed within one year (or the normal operating cycle, if longer). Assets are probable future economic benefits obtained or controlled by an entity as a result of past transactions or events.</t>
   </si>
   <si>
@@ -140,15 +131,6 @@
     <t>Carrying value as of the balance sheet date of obligations incurred and payable for statutory income, sales, use, payroll, excise, real, property and other taxes. Used to reflect the current portion of the liabilities (due within one year or within the normal operating cycle if longer).</t>
   </si>
   <si>
-    <t>Commercial papers</t>
-  </si>
-  <si>
-    <t>Commercial Paper</t>
-  </si>
-  <si>
-    <t>Carrying value as of the balance sheet date of short-term borrowings using unsecured obligations issued by banks, corporations and other borrowers to investors. The maturities of these money market securities generally do not exceed 270 days</t>
-  </si>
-  <si>
     <t>Operating Lease, Liability, Current</t>
   </si>
   <si>
@@ -164,15 +146,9 @@
     <t>Operating Lease, Liability, Non Current</t>
   </si>
   <si>
-    <t>Finance Lease, Liability, Non Current</t>
-  </si>
-  <si>
     <t>Total Assets</t>
   </si>
   <si>
-    <t>Sum of the carrying amounts as of the balance sheet date of all assets that are recognized. Assets are probable future economic benefits obtained or controlled by an entity as a result of past transactions or events</t>
-  </si>
-  <si>
     <t>Assets</t>
   </si>
   <si>
@@ -194,33 +170,18 @@
     <t>Accumulated Other Comprehensive Income (Loss), Net of Tax</t>
   </si>
   <si>
-    <t>Liabilities and Equity</t>
-  </si>
-  <si>
     <t>Preferred Stock</t>
   </si>
   <si>
-    <t>Accumulated change in equity from transactions and other events and circumstances from non-owner sources, net of tax effect, at period end. Excludes Net Income (Loss), and accumulated changes in equity from transactions resulting from investments by owners and distributions to owners. Includes foreign currency translation items, certain pension adjustments, unrealized gains and losses on certain investments in debt and equity securities, other than temporary impairment (OTTI) losses related to factors other than credit losses on available-for-sale and held-to-maturity debt securities that an entity does not intend to sell and it is not more likely than not that the entity will be required to sell before recovery of the amortized cost basis, as well as changes in the fair value of derivatives related to the effective portion of a designated cash flow hedge</t>
-  </si>
-  <si>
     <t>Amount of liabilities and equity items, including the portion of equity attributable to noncontrolling interests, if any.</t>
   </si>
   <si>
     <t>Cash &amp; Cash Equivalent</t>
   </si>
   <si>
-    <t>Total Long Term Liabilities</t>
-  </si>
-  <si>
     <t>Long Term Debt, Current Maturities</t>
   </si>
   <si>
-    <t>Amount, after unamortized (discount) premium and debt issuance costs, of Long Term debt, classified as current. Includes, but not limited to, notes payable, bonds payable, debentures, mortgage loans and commercial paper. Excludes capital lease obligations</t>
-  </si>
-  <si>
-    <t>Long Term Debts</t>
-  </si>
-  <si>
     <t>Long Term Debt, Excluding Current Maturities</t>
   </si>
   <si>
@@ -233,18 +194,9 @@
     <t>Assets, Non Current</t>
   </si>
   <si>
-    <t>Amount after unamortized (discount) premium and debt issuance costs of Long Term debt classified as Non Current and excluding amounts to be repaid within one year or the normal operating cycle, if longer. Includes, but not limited to, notes payable, bonds payable, debentures, mortgage loans and commercial paper. Excludes capital lease obligation</t>
-  </si>
-  <si>
     <t>Liabilities, Non Current</t>
   </si>
   <si>
-    <t>Carrying value as of the balance sheet date of liabilities incurred (and for which invoices have typically been received) and payable to vendors for goods and services received that are used in an entitys business. Used to reflect the current portion of the liabilities (due within one year or within the normal operating cycle if longer)</t>
-  </si>
-  <si>
-    <t>Present value of lessees discounted obligation for lease payments from operating lease, classified as current.</t>
-  </si>
-  <si>
     <t>Present value of lessees discounted obligation for lease payments from finance lease, classified as current.</t>
   </si>
   <si>
@@ -254,9 +206,6 @@
     <t>Present value of lessees discounted obligation for lease payments from finance lease, classified as Non Current.</t>
   </si>
   <si>
-    <t>The cumulative amount of the reporting entitys undistributed earnings or deficit.</t>
-  </si>
-  <si>
     <t>Stockholders Equity Attributable to Noncontrolling Interest</t>
   </si>
   <si>
@@ -269,9 +218,6 @@
     <t>Stockholders Equity, Including Portion Attributable to Noncontrolling Interest</t>
   </si>
   <si>
-    <t>Total Liabilities, preferred stock &amp; Stockholders Equity</t>
-  </si>
-  <si>
     <t>Preferred Stock, Shares Outstanding</t>
   </si>
   <si>
@@ -285,13 +231,73 @@
   </si>
   <si>
     <t>Short Term Debt</t>
+  </si>
+  <si>
+    <t>Marketable Securities Current</t>
+  </si>
+  <si>
+    <t>Marketable Securities Non Current</t>
+  </si>
+  <si>
+    <t>Property Plant and Equipment</t>
+  </si>
+  <si>
+    <t>Operating Lease Liability Current</t>
+  </si>
+  <si>
+    <t>Finance Lease Liability Current</t>
+  </si>
+  <si>
+    <t>Operating Lease Liability Non Current</t>
+  </si>
+  <si>
+    <t>Finance Lease Liability Non Current</t>
+  </si>
+  <si>
+    <t>Total Non Current Assets</t>
+  </si>
+  <si>
+    <t>Non Current Debts</t>
+  </si>
+  <si>
+    <t>Total Non Current Liabilities</t>
+  </si>
+  <si>
+    <t>Total Liabilities &amp; Stockholders Equity</t>
+  </si>
+  <si>
+    <t>Amount after valuation and LIFO reserves of inventory expected to be sold, or consumed within one year or operating cycle, if longer.</t>
+  </si>
+  <si>
+    <t>Sum of the carrying amounts as of the balance sheet date of all assets that are recognized. Assets are probable future economic benefits obtained or controlled by an entity as a result of past transactions or events.</t>
+  </si>
+  <si>
+    <t>Carrying value as of the balance sheet date of liabilities incurred (and for which invoices have typically been received) and payable to vendors for goods and services received that are used in an entity's business. Used to reflect the current portion of the liabilities (due within one year or within the normal operating cycle if longer).</t>
+  </si>
+  <si>
+    <t>Amount, after unamortized (discount) premium and debt issuance costs, of Long Term debt, classified as current. Includes, but not limited to, notes payable, bonds payable, debentures, mortgage loans and commercial paper. Excludes capital lease obligations.</t>
+  </si>
+  <si>
+    <t>Present value of lessee's discounted obligation for lease payments from operating lease, classified as current.</t>
+  </si>
+  <si>
+    <t>Amount after unamortized (discount) premium and debt issuance costs of Long Term debt classified as Non Current and excluding amounts to be repaid within one year or the normal operating cycle, if longer. Includes, but not limited to, notes payable, bonds payable, debentures, mortgage loans and commercial paper. Excludes capital lease obligation.</t>
+  </si>
+  <si>
+    <t>The cumulative amount of the reporting entity's undistributed earnings or deficit.</t>
+  </si>
+  <si>
+    <t>Accumulated change in equity from transactions and other events and circumstances from non-owner sources, net of tax effect, at period end. Excludes Net Income (Loss), and accumulated changes in equity from transactions resulting from investments by owners and distributions to owners. Includes foreign currency translation items, certain pension adjustments, unrealized gains and losses on certain investments in debt and equity securities, other than temporary impairment (OTTI) losses related to factors other than credit losses on available-for-sale and held-to-maturity debt securities that an entity does not intend to sell and it is not more likely than not that the entity will be required to sell before recovery of the amortized cost basis, as well as changes in the fair value of derivatives related to the effective portion of a designated cash flow hedge.</t>
+  </si>
+  <si>
+    <t>Liabilities and Equity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -306,19 +312,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Grande"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Grande"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -341,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -354,12 +347,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -676,16 +663,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="62.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="63.1640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="83.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="3" customWidth="1"/>
     <col min="8" max="8" width="65.33203125" customWidth="1"/>
@@ -696,57 +683,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>56</v>
+      <c r="A2" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>80</v>
+      <c r="A5" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -754,281 +741,270 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>62</v>
+      <c r="A7" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="B18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="C21" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>73</v>
+      <c r="A28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>76</v>
+      <c r="B29" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="D29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FactsList_to_Dataframe and standardized_balancesheet improvement
Improvement of FactsList_to_Dataframe function to incorporate the reference to us_gaap. Immproved standardized_balancesheet.xlsx (WIP)
</commit_message>
<xml_diff>
--- a/data/standardized_balancesheet.xlsx
+++ b/data/standardized_balancesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/SEC_data_analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/Documents/Github/SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922CA847-DB31-5D4F-816F-BEAFE993D958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7839B8-B0E8-2A49-BEAB-B01415B98FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="1600" windowWidth="21120" windowHeight="19980" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
+    <workbookView xWindow="13980" yWindow="860" windowWidth="20220" windowHeight="20000" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
   <si>
     <t>standardized_balancesheet_label</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Property, Plant and Equipment, Net</t>
   </si>
   <si>
-    <t>Cash and Cash Equivalents, at Carrying Value</t>
-  </si>
-  <si>
     <t>Marketable Securities, Current</t>
   </si>
   <si>
@@ -291,6 +288,48 @@
   </si>
   <si>
     <t>Liabilities and Equity</t>
+  </si>
+  <si>
+    <t>Cash and Cash Equivalents</t>
+  </si>
+  <si>
+    <t>Amount of cash and cash equivalents, and cash and cash equivalents restricted to withdrawal or usage. Excludes amount for disposal group and discontinued operations. Cash includes, but is not limited to, currency on hand, demand deposits with banks or financial institutions, and other accounts with general characteristics of demand deposits. Cash equivalents include, but are not limited to, short-term, highly liquid investments that are both readily convertible to known amounts of cash and so near their maturity that they present insignificant risk of changes in value because of changes in interest rates.</t>
+  </si>
+  <si>
+    <t>Cash Cash Equivalents Restricted Cash And Restricted Cash Equivalents</t>
+  </si>
+  <si>
+    <t>Amount of investment in marketable security, classified as current.</t>
+  </si>
+  <si>
+    <t>Prepaid Expenses</t>
+  </si>
+  <si>
+    <t>Other Current Assets</t>
+  </si>
+  <si>
+    <t>Other Assets, Current</t>
+  </si>
+  <si>
+    <t>Prepaid Expense, Current</t>
+  </si>
+  <si>
+    <t>Amount of asset related to consideration paid in advance for costs that provide economic benefits within a future period of one year or the normal operating cycle, if longer.</t>
+  </si>
+  <si>
+    <t>Other Assets, Current Amount of current assets classified as other.</t>
+  </si>
+  <si>
+    <t>Marketable Securities, Current Amount of investment in marketable security, classified as non current.</t>
+  </si>
+  <si>
+    <t>Molds and tooling, Net</t>
+  </si>
+  <si>
+    <t>Amount after accumulated depreciation of tangible personal property used to produce goods and services, including, but is not limited to, tools, dies and molds, computer and office equipment.</t>
+  </si>
+  <si>
+    <t>Operating Lease, Right-of-Use Asset</t>
   </si>
 </sst>
 </file>
@@ -314,12 +353,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -334,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -347,6 +392,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -663,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,7 +734,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="1"/>
@@ -694,317 +742,390 @@
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>14</v>
+      <c r="A6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>3</v>
+        <v>89</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>4</v>
+      <c r="A10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>51</v>
+      <c r="A11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>37</v>
+      <c r="A12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>94</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>30</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>69</v>
+      <c r="A17" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>48</v>
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>81</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="C25" s="4" t="s">
-        <v>82</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="4" t="s">
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="B35" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="2"/>
+      <c r="C35" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>